<commit_message>
Session 3 & 4
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>##</t>
   </si>
@@ -203,6 +203,56 @@
     <t>Jun 20 2023</t>
   </si>
   <si>
+    <t>Jayant, Himanshu, Shailendra, Vishal, Ankit G, Pavan</t>
+  </si>
+  <si>
+    <t>Devyani, Ashok, Nancy, Ankit J, Disha</t>
+  </si>
+  <si>
+    <t>Karate json response verification</t>
+  </si>
+  <si>
+    <t>* Matching individual data
+* Matching whole json object</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>* Manipulating data
+* Set single/multiple in json
+* remove in json
+* delete in json</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>* header verification
+* contains &amp; not-contains check</t>
+  </si>
+  <si>
+    <t>Jun 21 2023</t>
+  </si>
+  <si>
+    <t>Jayant, Himanshu, Shailendra, Vishal, Ankit G, Ankit J, Pavan, Ashok, Nancy</t>
+  </si>
+  <si>
+    <t>Devyani, Disha</t>
+  </si>
+  <si>
+    <t>* equality check using match
+* non-equality check using match
+* Fuzzy matching(dynamic)
+* Self validation expressions(javascript)</t>
+  </si>
+  <si>
+    <t>Assert</t>
+  </si>
+  <si>
     <t>Parallel Execution</t>
   </si>
   <si>
@@ -212,13 +262,10 @@
     <t>Scenario outline with example</t>
   </si>
   <si>
-    <t>Type / String coversion</t>
-  </si>
-  <si>
-    <t>Match</t>
-  </si>
-  <si>
-    <t>Assert</t>
+    <t>Type / String conversion</t>
+  </si>
+  <si>
+    <t>Calling other feature/scenarios</t>
   </si>
   <si>
     <t>Call</t>
@@ -229,10 +276,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -251,6 +298,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -267,23 +322,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -336,6 +382,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -344,6 +397,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -373,23 +434,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -410,19 +457,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,163 +631,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -601,21 +648,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -668,6 +700,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -704,49 +751,49 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -755,101 +802,101 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -858,6 +905,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1179,12 +1229,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -1194,7 +1244,7 @@
     <col min="4" max="4" width="82.8888888888889" style="2" customWidth="1"/>
     <col min="5" max="6" width="11.2222222222222" style="2" customWidth="1"/>
     <col min="7" max="7" width="27.6666666666667" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.8888888888889" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.2222222222222" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -1224,7 +1274,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="96" customHeight="1" spans="2:8">
+    <row r="2" ht="96" customHeight="1" spans="1:8">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1247,7 +1300,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" ht="86.4" spans="2:8">
+    <row r="3" ht="86.4" spans="1:8">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
@@ -1270,7 +1326,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="1:6">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1284,7 +1343,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" ht="100.8" spans="2:6">
+    <row r="5" ht="100.8" spans="1:6">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
@@ -1301,7 +1363,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" ht="28.8" spans="2:6">
+    <row r="6" ht="28.8" spans="1:6">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1318,7 +1383,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="1:6">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1332,7 +1400,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="1:6">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1346,7 +1417,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" ht="115.2" spans="2:6">
+    <row r="9" ht="115.2" spans="1:6">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1363,7 +1437,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="1:6">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1377,7 +1454,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" ht="57.6" spans="2:6">
+    <row r="11" ht="57.6" spans="1:6">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1394,7 +1474,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" ht="57.6" spans="2:5">
+    <row r="12" ht="57.6" spans="1:8">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
@@ -1407,40 +1490,136 @@
       <c r="E12" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="3:3">
+      <c r="F12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" ht="28.8" spans="1:6">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3">
+        <v>39</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" ht="57.6" spans="1:6">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3">
+        <v>41</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" ht="43.2" spans="1:8">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3">
+        <v>44</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" ht="57.6" spans="1:6">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="C16" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3">
+        <v>44</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
       <c r="C18" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3">
+      <c r="C26" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Session 4, 5, & 6 Codes
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
   <si>
     <t>##</t>
   </si>
@@ -250,15 +250,66 @@
 * Self validation expressions(javascript)</t>
   </si>
   <si>
-    <t>Assert</t>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>* Understading the LHS and RHS of the syntax
+* Schema validation
+* matching array length
+* match text or binary
+* match karate.lowerCase()</t>
+  </si>
+  <si>
+    <t>Jun 28 2023</t>
+  </si>
+  <si>
+    <t>Shailendra, Vishal, Ankit G, Ankit J, Pavan, Ashok</t>
+  </si>
+  <si>
+    <t>Devyani, Disha, Jayant, Himanshu, Nancy</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>* match contains only
+* match contains any
+* match each</t>
+  </si>
+  <si>
+    <t>Jul 4 2023</t>
+  </si>
+  <si>
+    <t>Jayant, Himanshu, Shailendra, Vishal, Ankit J, Pavan, Ashok</t>
+  </si>
+  <si>
+    <t>Ankit G, Nancy, Devyani, Disha, Nancy</t>
   </si>
   <si>
     <t>Parallel Execution</t>
   </si>
   <si>
+    <t>* run scenarios in parallel
+* ignore scenarios
+* set env</t>
+  </si>
+  <si>
+    <t>Passing headers in request</t>
+  </si>
+  <si>
+    <t>* Passing headers in request individually using key:value pairs
+* Passing headers in request as json
+* configure headers</t>
+  </si>
+  <si>
     <t>Config parameters</t>
   </si>
   <si>
+    <t>* set timeouts
+* set env
+* set global variable</t>
+  </si>
+  <si>
     <t>Scenario outline with example</t>
   </si>
   <si>
@@ -266,6 +317,9 @@
   </si>
   <si>
     <t>Calling other feature/scenarios</t>
+  </si>
+  <si>
+    <t>Dynamic data passing in request payload</t>
   </si>
   <si>
     <t>Call</t>
@@ -276,10 +330,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -298,6 +352,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -306,20 +381,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -329,7 +390,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -366,6 +427,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -382,13 +458,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -399,21 +468,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -428,15 +483,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -457,37 +511,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,145 +685,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,6 +702,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -693,23 +762,28 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -728,171 +802,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1232,9 +1286,9 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -1586,40 +1640,124 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="3:5">
+    <row r="17" ht="72" spans="1:8">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" ht="43.2" spans="1:8">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="3:3">
+        <v>44</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" ht="43.2" spans="1:6">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="C19" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3">
+        <v>60</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" ht="43.2" spans="1:5">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
       <c r="C20" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3">
+        <v>62</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" ht="43.2" spans="1:4">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
       <c r="C21" s="2" t="s">
-        <v>53</v>
+        <v>64</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="3:3">
       <c r="C23" s="2" t="s">
-        <v>55</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3">
+      <c r="C24" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3">
+      <c r="C25" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26" s="2" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>